<commit_message>
Data driven via excel
</commit_message>
<xml_diff>
--- a/E-Commerce/src/main/java/utilities/excelFile.xlsx
+++ b/E-Commerce/src/main/java/utilities/excelFile.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\OneDrive\Desktop\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{306F66BB-7957-40E3-A1A6-441C258FAF5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8979930A-CDC8-4A5B-8771-250C4B3753ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E5FDA2A7-5B04-4CE2-89B3-CA91837FCB45}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5FDA2A7-5B04-4CE2-89B3-CA91837FCB45}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ContactPage" sheetId="1" r:id="rId1"/>
+    <sheet name="LandingPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,36 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Name</t>
+    <t>CUSTOMER SERVICE - CONTACT US</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>Your message has been successfully sent to our team.</t>
   </si>
   <si>
-    <t>Mohit</t>
-  </si>
-  <si>
-    <t>Ankit</t>
-  </si>
-  <si>
-    <t>Nalin</t>
-  </si>
-  <si>
-    <t>Chintu</t>
-  </si>
-  <si>
-    <t>Ashu</t>
-  </si>
-  <si>
-    <t>Guddu</t>
-  </si>
-  <si>
-    <t>Anu</t>
-  </si>
-  <si>
-    <t>Mobile_Number</t>
+    <t>My Store</t>
   </si>
 </sst>
 </file>
@@ -415,76 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFBE8FB-9C7A-4A49-B2E1-7E6419C1A533}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -494,76 +417,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0120514-95C3-4935-B5BD-F565D95139E0}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>7000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>